<commit_message>
update with infineon excel
</commit_message>
<xml_diff>
--- a/server/InfineonMap.xlsx
+++ b/server/InfineonMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EsperSean\Pictures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nico/Documents/GitHub/infineonmap/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{102E7AC9-3176-4809-9FA5-7A31538D1D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3F55A5-EF02-0946-AA31-43557F389AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{F9CBE48B-C521-4DDC-87E9-48805B4EC46E}"/>
+    <workbookView xWindow="100" yWindow="600" windowWidth="51000" windowHeight="28100" xr2:uid="{F9CBE48B-C521-4DDC-87E9-48805B4EC46E}"/>
   </bookViews>
   <sheets>
     <sheet name="query (3)" sheetId="1" r:id="rId1"/>
@@ -720,57 +720,56 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -785,15 +784,15 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -827,9 +826,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{021CAB72-C640-4A99-826F-2BAF050D933A}" name="Table_query__3" displayName="Table_query__3" ref="A1:F10" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:F10" xr:uid="{021CAB72-C640-4A99-826F-2BAF050D933A}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{93426779-AD4F-4156-B267-97B4A6DDBC80}" uniqueName="Title" name="Bezeichnung des Ortes" queryTableFieldId="1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{8A676D72-7B2A-47CE-9634-D08714A3A720}" uniqueName="Geo_x005f_x002d_Koordinaten" name="Geo-Koordinaten" queryTableFieldId="2" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{C09159F0-FB04-4F30-88A9-D05BF92DF82C}" uniqueName="Kurze_x005f_x0020_Beschreibung" name="kurze Beschreibung / Begründung" queryTableFieldId="3" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{93426779-AD4F-4156-B267-97B4A6DDBC80}" uniqueName="Title" name="Bezeichnung des Ortes" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{8A676D72-7B2A-47CE-9634-D08714A3A720}" uniqueName="Geo_x005f_x002d_Koordinaten" name="Geo-Koordinaten" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{C09159F0-FB04-4F30-88A9-D05BF92DF82C}" uniqueName="Kurze_x005f_x0020_Beschreibung" name="kurze Beschreibung / Begründung" queryTableFieldId="3" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{DE65A668-63F7-4957-B807-CBC48BCFFB7A}" uniqueName="Author" name="Created By" queryTableFieldId="4" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{048C83AD-EDF8-4B34-A370-53DE2707B4EA}" uniqueName="FSObjType" name="Item Type" queryTableFieldId="6" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{724017CB-A950-4D7E-B0D4-C7C52DF645A6}" uniqueName="FileDirRef" name="Path" queryTableFieldId="5" dataDxfId="0"/>
@@ -839,7 +838,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1157,19 +1156,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD8AF4E-7BEF-4CFC-B140-E5957A51D4D1}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1189,7 +1190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="272" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1199,7 +1200,7 @@
       <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1209,7 +1210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="176" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1219,7 +1220,7 @@
       <c r="C3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -1229,7 +1230,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="406" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1239,7 +1240,7 @@
       <c r="C4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -1249,7 +1250,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="288" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -1259,7 +1260,7 @@
       <c r="C5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -1269,7 +1270,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="176" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -1279,7 +1280,7 @@
       <c r="C6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -1289,7 +1290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1299,7 +1300,7 @@
       <c r="C7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1309,7 +1310,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="203" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1319,7 +1320,7 @@
       <c r="C8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -1329,7 +1330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1339,7 +1340,7 @@
       <c r="C9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -1349,7 +1350,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="319" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="335" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -1359,7 +1360,7 @@
       <c r="C10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="2" t="s">

</xml_diff>

<commit_message>
Nico Changes Location Fixes
</commit_message>
<xml_diff>
--- a/server/InfineonMap.xlsx
+++ b/server/InfineonMap.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nico/Documents/GitHub/infineonmap/server/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EsperSean\Documents\DevApps\ReactApps\infineonmap\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3F55A5-EF02-0946-AA31-43557F389AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A313D6ED-4BE2-452B-AA29-571443A2890C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="600" windowWidth="51000" windowHeight="28100" xr2:uid="{F9CBE48B-C521-4DDC-87E9-48805B4EC46E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{F9CBE48B-C521-4DDC-87E9-48805B4EC46E}"/>
   </bookViews>
   <sheets>
     <sheet name="query (3)" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="query__3" localSheetId="0" hidden="1">'query (3)'!$A$1:$F$10</definedName>
+    <definedName name="query__3" localSheetId="0" hidden="1">'query (3)'!$A$1:$F$15</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>Bezeichnung des Ortes</t>
   </si>
@@ -51,15 +51,9 @@
     <t>Item Type</t>
   </si>
   <si>
-    <t>Cafe Boot in Mariaort</t>
-  </si>
-  <si>
     <t>49.01898798697924, 12.031404677911548</t>
   </si>
   <si>
-    <t>Benkert Michael (BE R QM)</t>
-  </si>
-  <si>
     <t>sites/Lieblingsplaetze/Lists/Mein Favorit</t>
   </si>
   <si>
@@ -81,9 +75,6 @@
     <t>49.018260, 12.092114</t>
   </si>
   <si>
-    <t>Sessler Wolfgang (CSC FI MEA ANA DS)</t>
-  </si>
-  <si>
     <t>Marc-Aurel-Ufer, Regensburg</t>
   </si>
   <si>
@@ -117,9 +108,6 @@
     <t>49.02708799815702, 12.076379305724535</t>
   </si>
   <si>
-    <t>Gruenewald Clemens (FE QM FA RBG 1)</t>
-  </si>
-  <si>
     <t>Toller Ausblick auf Regenstauf</t>
   </si>
   <si>
@@ -133,9 +121,6 @@
   </si>
   <si>
     <t>48.93644130194383, 12.040389229543164</t>
-  </si>
-  <si>
-    <t>Zirngibl Wolfgang (FE RBG QM QF AUDIT)</t>
   </si>
   <si>
     <t xml:space="preserve">Im Café Boot, welches zum Kanuverleih "Paddelzeit" gehört, heißt es ankommen und den Urlaubsmodus anschalten. Das liebevoll eingerichteteCafé​ bietet nicht nur Kaffee und Kuchen, sondern auch viele weitere antialkoholische und alkoholische Getränke an – sowie Eis :-)
@@ -152,26 +137,104 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Wer es mal ruhig und auch mal sehr wuselig mag, ist auf einer der Bänke am Marc-Aurel-Ufer entlang der Donau bestens aufgehoben. Hier kommen Einheimische ("Schön, Dich zu sehen!") ebenso vorbei, wie Menschen aus allen Ländern ("How do I get to the cathedral, please?​"). Es​ ist eine Gesamtschau des Typen Mensch und von Hunderassen. Die fahrenden Schiffe wie die festgemachten des Schifffahrtsmuseums bieten auch Abwechslung. Und das Beste: Gleich auf der anderen Straßenseite gibt es im Aamu bestes Eis und Kaffee, auch zum Mitnehmen (und Wiederbringen) in der Tasse.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Der Spielplatz liegt versteckt, umringt von Gärten, mitten im Wohngebiet. Kinder können hier frei spielen, ohne Autos oder Durchgangsverkehr. Viele Bäume bieten im Sommer Schatten. Ein nett angelegter Sandkasten mit Wasserpumpe für die Kleinen, ein Klettergerüst mit Rutsche für die Größeren. Eine Eisdiele gibt es auch in der Nähe.
 </t>
   </si>
   <si>
-    <t xml:space="preserve">In Mitten von Feldern,​ umrahmt von Wald, Bayernfahne und "​Bavaria Blue Sky": Die Kapelle auf dem Affeckinger Berg in Kelheim ist ein magischer Ort.
-Dort findet man die Ruhe und Besinnung auf das Wesentliche.  Himmel und Erde ​sind gleichzeitig nicht nur optisch zu erleben; es schärft die Sinne, mitten in der Natur zu sein.Rund herum mit einer Wiese voller Leben​​​ – Insekten,kleinen Reptilien und Vögeln. Das ist im wahrsten Sinne einfach natürlich.​​
+    <t xml:space="preserve">Das Hochwasser im Sommer 2024 hat überraschend am Pfaffensteiner Wehr eine neue, kleine Halbinsel in der Donau zurückgelassen. Ein kleiner Sandstrand, den es vorher nicht gab. Dort konnte man vor dem Hochwasser nachts Biber beobachten, wie sie Zweige sammeln. J​etzt sitzen dort Angler und menschliche Baumeister, die aus Ästen spielerisch einen Unterstand gebaut haben.
+</t>
+  </si>
+  <si>
+    <t>Herzogspark</t>
+  </si>
+  <si>
+    <t>49.02329295165495, 12.081961310138482</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Willkommen im Herzogspark – meinem Lieblingsort in Regensburg. Mit seinen 1,5 Hektar bezaubernder Landschaftsarchitektur, einer Vielfalt an botanischen Schätzen und zahlreichen Sitzgelegenheiten bietet der Herzogspark eine nahezu magische und friedvolle Atmosphäre. Ein Spaziergang durch den Park führt nicht nur zur Entspannung, sondern auch zur Entdeckung vieler exotischer Pflanzen, die mit kleinen Schildern versehen sind. Der Renaissancegarten, der Rosengarten und der idyllische Teich, oben auf dem Hügel des Herzogsparks, sind meine persönlichen Highlights. ​
+</t>
+  </si>
+  <si>
+    <t>Giuzio Jasmin Gelsomina (FE RBG C)</t>
+  </si>
+  <si>
+    <t>Winzerer Höhen (Aussichtsbank)</t>
+  </si>
+  <si>
+    <t>49.035217644763904, 12.058639391094259</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeder kennt's: Am Meer in die Weite blicken und dabei die Seele baumeln lassen. Das befreit und macht glücklich. Nun liegt Regensburg leider nicht am Meer und dennoch gibt es einen Ort, der ähnliche Weite und Gefühle zulässt. Die Aussicht von den Winzerer Höhen über Regensburg. Dorthin spazieren, hinsetzen und tief durchatmen und dabei mit dem Blick in die Weite über unsere wunderschöne Stadt und die Donau einfach mal die Seele baumeln lassen. Das ist Kurzurlaub für Seele und Gemüt.​
+</t>
+  </si>
+  <si>
+    <t>Stich Andrea (FE CF QM ACA)</t>
+  </si>
+  <si>
+    <t>Lerautal und Burg Leuchtenberg</t>
+  </si>
+  <si>
+    <t>49.60386, 12.26682</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bei jeder Reise von Regensburg aus in Richtung Norden, lohnt sich ein Abstecher in das wunderbare​ Lerautal ... Von der kurzen Auszeit bis hin zum Tagesausflug ist hier alles möglich. Wandern, klettern, planschen, die Ruhe genießen, Abenteuer erleben, Naturdenkmäler entdecken sowie​ Geschichte in der Burg Leuchtenberg hautnah erleben. Vm Wanderparkplatz an der Bundesstraße 22 aus ist der Lerautal-Rundwanderweg ein Erlebnis für die ganze Familie!
+</t>
+  </si>
+  <si>
+    <t>Gallersdoerfer Tobias (BE RBG OP LC)</t>
+  </si>
+  <si>
+    <t>Bismarckplatz</t>
+  </si>
+  <si>
+    <t>49.01876103303881, 12.089595118683107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einfach und schön - der Bismarckplatz in der Altstadt. Vor allem an warmen Sommertagen kann man hier sehr gut seine Zeit verbringen, ein Eis essen oder sich bei einem der naheliegenden Café​s einen Aperol Spritz bestellen. Der perfekte Ort, um alleine eine kurze Pause zu machen oder sich mit Freunden zu treffen. 
+</t>
+  </si>
+  <si>
+    <t>Dorner Andrea (FE RBG C)</t>
+  </si>
+  <si>
+    <t>Malefiz</t>
+  </si>
+  <si>
+    <t>49.0175109155855, 12.096109231457973</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gutes Essen, nette Bedienung - was will man mehr? Probiert's aus!
+</t>
+  </si>
+  <si>
+    <t>Goetz Sabrina (FE RBG C)</t>
+  </si>
+  <si>
+    <t>Café Boot in Mariaort</t>
+  </si>
+  <si>
+    <t>Benkert Michael (BE QM PP RBG)</t>
+  </si>
+  <si>
+    <t>Sessler Wolfgang (CSC FI MDI EPA STA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wer es mal ruhig und auch mal sehr wuselig mag, ist auf einer der Bänke am Marc-Aurel-Ufer entlang der Donau bestens aufgehoben. Hier kommen Einheimische ("​Schön, Dich zu sehen!") ebenso vorbei, wie Menschen aus allen Ländern ("How do I get to the cathedral, please?​"). Es​ ist eine Gesamtschau des Typen Mensch und von Hunderassen. Die fahrenden Schiffe wie die festgemachten des Schifffahrtsmuseums bieten auch Abwechslung. Und das Beste: Gleich auf der anderen Straßenseite gibt es im Aamu bestes Eis und Kaffee, auch zum Mitnehmen (und Wiederbringen) in der Tasse.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inmitten von Feldern,​ umrahmt von Wald, Bayernfahne und "​Bavaria Blue Sky": Die Kapelle auf dem Affeckinger Berg in Kelheim ist ein magischer Ort.
+Dort findet man die Ruhe und Besinnung auf das Wesentliche.  Himmel und Erde ​sind gleichzeitig nicht nur optisch zu erleben; es schärft die Sinne, mitten in der Natur zu sein.Rundherum mit einer Wiese voller Leben​​​ – Insekten,kleinen Reptilien und Vögeln. Das ist im wahrsten Sinne einfach natürlich.​​
 Auch die Tiere des Waldes lassen sich hin und wieder und nach Tageszeit auf den Feldern sehen, umrahmt von Wald,​ wie auf einem gemalten Bild. Der Ort gibt einem die Energie wieder, die uns der Alltag abfordert. Der Trubel der Städte liegt hier hinter uns - es ist ein Ort des Friedens.
 Gleichzeitig mahnt es uns, in Einklang mit der Natur zu leben, damit uns unsere Heimat und "Mutter Erde" erhalten bleibt.
+​
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Das Hochwasser im Sommer 2024 hat überraschend am Pfaffensteiner Wehr eine neue, kleine Halbinsel in der Donau zurückgelassen. Ein kleiner Sandstrand, den es vorher nicht gab. Dort konnte man vor dem Hochwasser nachts Biber beobachten, wie sie Zweige sammeln. J​etzt sitzen dort Angler und menschliche Baumeister, die aus Ästen spielerisch einen Unterstand gebaut haben.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ein meist ruhiges Plätzens - vor allem am Abend sehr schön sich den Wund um die Nase wehen zu lassen. Es gibt von dort einen tollen Ausblick auf Regenstauf.
+    <t>Gruenewald Clemens (FE CF QM FA RBG 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ein meist ruhiges Plätzchen – vor allem am Abend ist es sehr schön, um sich den Wi​​nd um die Nase wehen zu lassen. Es gibt von dort einen tollen Ausblick auf Regenstauf.
 </t>
   </si>
   <si>
@@ -186,8 +249,7 @@
         <color theme="1"/>
         <rFont val="Aptos Narrow"/>
       </rPr>
-      <t xml:space="preserve">Entdecken Sie bayerische Gaumenfreuden im Gasthaus Zirngibl in Bad Abbach
-</t>
+      <t>Entdecken Sie bayerische Gaumenfreuden im Gasthaus Zirngibl in Bad Abbach. </t>
     </r>
     <r>
       <rPr>
@@ -197,40 +259,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Nur wenige Kilometer von Regensburg entfernt, steht das Gasthaus Zirngibl in Bad Abbach als Zeugnis bayerischer Tradition. Gut mit dem Fahrrad zu erreichen.
+      <t xml:space="preserve">Nur wenige Kilometer von Regensburg entfernt steht das Gasthaus Zirngibl in Bad Abbach als Zeugnis bayerischer Tradition. Es ist g​ut mit dem Fahrrad zu erreichen. Sie werden mit einem freundlichen Lächeln und von einer Speisekarte begrüßt, die voller bayerischer Köstlichkeiten steckt. Auch spontane Besuche sind kein Problem. Die großzügigen Portionen garantieren, dass niemand hungrig nach Hause geht. Es ist ein kulinarisches Ziel, das man besucht haben muss​.
 </t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t xml:space="preserve">Unvergleichliche Gastfreundschaft und Service
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Sie werden mit einem freundlichen Lächeln und einer Speisekarte begrüßt, die voller bayerischer Köstlichkeiten steckt. Auch spontane Besuche sind kein Problem. Die großzügigen Portionen garantieren, dass niemand hungrig nach Hause geht.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t xml:space="preserve">Ein kulinarisches Ziel, das man besucht haben muss​
-</t>
-    </r>
+  </si>
+  <si>
+    <t>Zirngibl Wolfgang (FE CF QM RBG QF AUDIT)</t>
   </si>
 </sst>
 </file>
@@ -728,50 +762,53 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -823,22 +860,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{021CAB72-C640-4A99-826F-2BAF050D933A}" name="Table_query__3" displayName="Table_query__3" ref="A1:F10" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:F10" xr:uid="{021CAB72-C640-4A99-826F-2BAF050D933A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{021CAB72-C640-4A99-826F-2BAF050D933A}" name="Table_query__3" displayName="Table_query__3" ref="A1:F15" tableType="queryTable" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:F15" xr:uid="{021CAB72-C640-4A99-826F-2BAF050D933A}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{93426779-AD4F-4156-B267-97B4A6DDBC80}" uniqueName="Title" name="Bezeichnung des Ortes" queryTableFieldId="1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{8A676D72-7B2A-47CE-9634-D08714A3A720}" uniqueName="Geo_x005f_x002d_Koordinaten" name="Geo-Koordinaten" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{C09159F0-FB04-4F30-88A9-D05BF92DF82C}" uniqueName="Kurze_x005f_x0020_Beschreibung" name="kurze Beschreibung / Begründung" queryTableFieldId="3" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{DE65A668-63F7-4957-B807-CBC48BCFFB7A}" uniqueName="Author" name="Created By" queryTableFieldId="4" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{048C83AD-EDF8-4B34-A370-53DE2707B4EA}" uniqueName="FSObjType" name="Item Type" queryTableFieldId="6" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{724017CB-A950-4D7E-B0D4-C7C52DF645A6}" uniqueName="FileDirRef" name="Path" queryTableFieldId="5" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{93426779-AD4F-4156-B267-97B4A6DDBC80}" uniqueName="Title" name="Bezeichnung des Ortes" queryTableFieldId="1" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{8A676D72-7B2A-47CE-9634-D08714A3A720}" uniqueName="Geo_x005f_x002d_Koordinaten" name="Geo-Koordinaten" queryTableFieldId="2" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{C09159F0-FB04-4F30-88A9-D05BF92DF82C}" uniqueName="Kurze_x005f_x0020_Beschreibung" name="kurze Beschreibung / Begründung" queryTableFieldId="3" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{DE65A668-63F7-4957-B807-CBC48BCFFB7A}" uniqueName="Author" name="Created By" queryTableFieldId="4" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{048C83AD-EDF8-4B34-A370-53DE2707B4EA}" uniqueName="FSObjType" name="Item Type" queryTableFieldId="6" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{724017CB-A950-4D7E-B0D4-C7C52DF645A6}" uniqueName="FileDirRef" name="Path" queryTableFieldId="5" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1154,23 +1191,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD8AF4E-7BEF-4CFC-B140-E5957A51D4D1}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1190,184 +1227,284 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="272" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="406" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="203" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="261" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
+      <c r="F11" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="176" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>9</v>
+    <row r="12" spans="1:6" ht="232" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
+    <row r="13" spans="1:6" ht="232" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="288" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
+    <row r="14" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="176" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="192" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="96" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="335" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>9</v>
+    <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>